<commit_message>
Fix error with exclude column in the meta output by running with --update-expected-files
</commit_message>
<xml_diff>
--- a/tests/test-data/workflow-ciceroscm-slimmed/ex2_full_exceedance_probabilities.xlsx
+++ b/tests/test-data/workflow-ciceroscm-slimmed/ex2_full_exceedance_probabilities.xlsx
@@ -663,40 +663,40 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1.261653289019607</v>
+        <v>1.261653194362745</v>
       </c>
       <c r="M2">
-        <v>1.265592726470588</v>
+        <v>1.265592636078431</v>
       </c>
       <c r="N2">
-        <v>1.271107938901961</v>
+        <v>1.271107854480392</v>
       </c>
       <c r="O2">
-        <v>1.302179174558824</v>
+        <v>1.302179074313726</v>
       </c>
       <c r="P2">
-        <v>1.348111291656863</v>
+        <v>1.348111162</v>
       </c>
       <c r="Q2">
-        <v>1.416934373529412</v>
+        <v>1.41693424754902</v>
       </c>
       <c r="R2">
-        <v>1.481424518823529</v>
+        <v>1.481424422843137</v>
       </c>
       <c r="S2">
-        <v>1.487400796470588</v>
+        <v>1.487400700588235</v>
       </c>
       <c r="T2">
-        <v>1.535211017647059</v>
+        <v>1.53521092254902</v>
       </c>
       <c r="U2">
-        <v>1.567951840882353</v>
+        <v>1.567951758039216</v>
       </c>
       <c r="V2">
-        <v>1.574623855882353</v>
+        <v>1.574623800490196</v>
       </c>
       <c r="W2">
-        <v>1.579389580882353</v>
+        <v>1.579389545098039</v>
       </c>
       <c r="X2">
         <v>2048</v>
@@ -770,40 +770,40 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>1.260918289019608</v>
+        <v>1.260918194362745</v>
       </c>
       <c r="M3">
-        <v>1.264802726470588</v>
+        <v>1.264802636078432</v>
       </c>
       <c r="N3">
-        <v>1.270240938901961</v>
+        <v>1.270240854480392</v>
       </c>
       <c r="O3">
-        <v>1.301221674558824</v>
+        <v>1.301221574313726</v>
       </c>
       <c r="P3">
-        <v>1.347061791656863</v>
+        <v>1.347061662</v>
       </c>
       <c r="Q3">
-        <v>1.415839373529412</v>
+        <v>1.41583924754902</v>
       </c>
       <c r="R3">
-        <v>1.480130518823529</v>
+        <v>1.480130422843137</v>
       </c>
       <c r="S3">
-        <v>1.486067796470588</v>
+        <v>1.486067700588236</v>
       </c>
       <c r="T3">
-        <v>1.533566017647059</v>
+        <v>1.53356592254902</v>
       </c>
       <c r="U3">
-        <v>1.566243840882353</v>
+        <v>1.566243758039216</v>
       </c>
       <c r="V3">
-        <v>1.573223855882353</v>
+        <v>1.573223800490196</v>
       </c>
       <c r="W3">
-        <v>1.578209580882353</v>
+        <v>1.578209545098039</v>
       </c>
       <c r="X3">
         <v>2040</v>
@@ -877,40 +877,40 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1.256278289019608</v>
+        <v>1.256278194362745</v>
       </c>
       <c r="M4">
-        <v>1.260012726470588</v>
+        <v>1.260012636078431</v>
       </c>
       <c r="N4">
-        <v>1.265240938901961</v>
+        <v>1.265240854480392</v>
       </c>
       <c r="O4">
-        <v>1.295456674558824</v>
+        <v>1.295456574313726</v>
       </c>
       <c r="P4">
-        <v>1.340216791656863</v>
+        <v>1.340216662</v>
       </c>
       <c r="Q4">
-        <v>1.407954373529412</v>
+        <v>1.40795424754902</v>
       </c>
       <c r="R4">
-        <v>1.47179951882353</v>
+        <v>1.471799422843138</v>
       </c>
       <c r="S4">
-        <v>1.477678296470588</v>
+        <v>1.477678200588236</v>
       </c>
       <c r="T4">
-        <v>1.524708517647059</v>
+        <v>1.52470842254902</v>
       </c>
       <c r="U4">
-        <v>1.557156840882353</v>
+        <v>1.557156758039216</v>
       </c>
       <c r="V4">
-        <v>1.564283855882353</v>
+        <v>1.564283800490196</v>
       </c>
       <c r="W4">
-        <v>1.569374580882353</v>
+        <v>1.569374545098039</v>
       </c>
       <c r="X4">
         <v>2038</v>
@@ -984,40 +984,40 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>1.278835789019608</v>
+        <v>1.278835694362745</v>
       </c>
       <c r="M5">
-        <v>1.282857726470588</v>
+        <v>1.282857636078431</v>
       </c>
       <c r="N5">
-        <v>1.288488438901961</v>
+        <v>1.288488354480392</v>
       </c>
       <c r="O5">
-        <v>1.320071674558824</v>
+        <v>1.320071574313726</v>
       </c>
       <c r="P5">
-        <v>1.366743791656863</v>
+        <v>1.366743662</v>
       </c>
       <c r="Q5">
-        <v>1.436479373529412</v>
+        <v>1.43647924754902</v>
       </c>
       <c r="R5">
-        <v>1.50200851882353</v>
+        <v>1.502008422843137</v>
       </c>
       <c r="S5">
-        <v>1.508113796470588</v>
+        <v>1.508113700588235</v>
       </c>
       <c r="T5">
-        <v>1.556956017647059</v>
+        <v>1.55695592254902</v>
       </c>
       <c r="U5">
-        <v>1.590257840882353</v>
+        <v>1.590257758039216</v>
       </c>
       <c r="V5">
-        <v>1.596733855882353</v>
+        <v>1.596733800490196</v>
       </c>
       <c r="W5">
-        <v>1.601359580882353</v>
+        <v>1.601359545098039</v>
       </c>
       <c r="X5">
         <v>2048</v>
@@ -1091,40 +1091,40 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>1.256278289019608</v>
+        <v>1.256278194362745</v>
       </c>
       <c r="M6">
-        <v>1.260012726470588</v>
+        <v>1.260012636078431</v>
       </c>
       <c r="N6">
-        <v>1.265240938901961</v>
+        <v>1.265240854480392</v>
       </c>
       <c r="O6">
-        <v>1.295456674558824</v>
+        <v>1.295456574313726</v>
       </c>
       <c r="P6">
-        <v>1.340216791656863</v>
+        <v>1.340216662</v>
       </c>
       <c r="Q6">
-        <v>1.407954373529412</v>
+        <v>1.40795424754902</v>
       </c>
       <c r="R6">
-        <v>1.47179951882353</v>
+        <v>1.471799422843138</v>
       </c>
       <c r="S6">
-        <v>1.477678296470588</v>
+        <v>1.477678200588236</v>
       </c>
       <c r="T6">
-        <v>1.524708517647059</v>
+        <v>1.52470842254902</v>
       </c>
       <c r="U6">
-        <v>1.557156840882353</v>
+        <v>1.557156758039216</v>
       </c>
       <c r="V6">
-        <v>1.564283855882353</v>
+        <v>1.564283800490196</v>
       </c>
       <c r="W6">
-        <v>1.569374580882353</v>
+        <v>1.569374545098039</v>
       </c>
       <c r="X6">
         <v>2038</v>
@@ -1198,40 +1198,40 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>1.256523289019608</v>
+        <v>1.256523194362745</v>
       </c>
       <c r="M7">
-        <v>1.260612726470588</v>
+        <v>1.260612636078431</v>
       </c>
       <c r="N7">
-        <v>1.266337938901961</v>
+        <v>1.266337854480392</v>
       </c>
       <c r="O7">
-        <v>1.298519174558824</v>
+        <v>1.298519074313726</v>
       </c>
       <c r="P7">
-        <v>1.346083291656863</v>
+        <v>1.346083162</v>
       </c>
       <c r="Q7">
-        <v>1.417904373529412</v>
+        <v>1.41790424754902</v>
       </c>
       <c r="R7">
-        <v>1.48697951882353</v>
+        <v>1.486979422843137</v>
       </c>
       <c r="S7">
-        <v>1.493458296470588</v>
+        <v>1.493458200588236</v>
       </c>
       <c r="T7">
-        <v>1.545288517647059</v>
+        <v>1.54528842254902</v>
       </c>
       <c r="U7">
-        <v>1.580195340882353</v>
+        <v>1.580195258039216</v>
       </c>
       <c r="V7">
-        <v>1.586058855882353</v>
+        <v>1.586058800490196</v>
       </c>
       <c r="W7">
-        <v>1.590247080882353</v>
+        <v>1.590247045098039</v>
       </c>
       <c r="X7">
         <v>2040</v>
@@ -1305,40 +1305,40 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>1.347640789019608</v>
+        <v>1.347638194362745</v>
       </c>
       <c r="M8">
-        <v>1.352427726470588</v>
+        <v>1.352422636078431</v>
       </c>
       <c r="N8">
-        <v>1.359129438901961</v>
+        <v>1.359120854480392</v>
       </c>
       <c r="O8">
-        <v>1.394126674558823</v>
+        <v>1.394119074313725</v>
       </c>
       <c r="P8">
-        <v>1.445526791656863</v>
+        <v>1.445523162</v>
       </c>
       <c r="Q8">
-        <v>1.521589373529412</v>
+        <v>1.52158924754902</v>
       </c>
       <c r="R8">
-        <v>1.596046518823529</v>
+        <v>1.596046422843137</v>
       </c>
       <c r="S8">
-        <v>1.603274796470588</v>
+        <v>1.603274700588235</v>
       </c>
       <c r="T8">
-        <v>1.661101017647059</v>
+        <v>1.66110092254902</v>
       </c>
       <c r="U8">
-        <v>1.698780340882353</v>
+        <v>1.698780258039216</v>
       </c>
       <c r="V8">
-        <v>1.702368855882353</v>
+        <v>1.702368800490196</v>
       </c>
       <c r="W8">
-        <v>1.704932080882353</v>
+        <v>1.704932045098039</v>
       </c>
       <c r="X8">
         <v>2048</v>
@@ -1412,40 +1412,40 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>1.229325789019608</v>
+        <v>1.229325694362745</v>
       </c>
       <c r="M9">
-        <v>1.232957726470588</v>
+        <v>1.232957636078432</v>
       </c>
       <c r="N9">
-        <v>1.238042438901961</v>
+        <v>1.238042354480392</v>
       </c>
       <c r="O9">
-        <v>1.267449174558823</v>
+        <v>1.267449074313725</v>
       </c>
       <c r="P9">
-        <v>1.311013291656863</v>
+        <v>1.311013162</v>
       </c>
       <c r="Q9">
-        <v>1.376539373529412</v>
+        <v>1.37653924754902</v>
       </c>
       <c r="R9">
-        <v>1.437029518823529</v>
+        <v>1.437029422843137</v>
       </c>
       <c r="S9">
-        <v>1.442543296470588</v>
+        <v>1.442543200588235</v>
       </c>
       <c r="T9">
-        <v>1.486653517647059</v>
+        <v>1.48665342254902</v>
       </c>
       <c r="U9">
-        <v>1.517525840882353</v>
+        <v>1.517525758039216</v>
       </c>
       <c r="V9">
-        <v>1.525233855882353</v>
+        <v>1.525233800490196</v>
       </c>
       <c r="W9">
-        <v>1.530739580882353</v>
+        <v>1.530739545098039</v>
       </c>
       <c r="X9">
         <v>2048</v>
@@ -1519,40 +1519,40 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>1.229315789019608</v>
+        <v>1.229315694362745</v>
       </c>
       <c r="M10">
-        <v>1.232947726470588</v>
+        <v>1.232947636078431</v>
       </c>
       <c r="N10">
-        <v>1.238032438901961</v>
+        <v>1.238032354480392</v>
       </c>
       <c r="O10">
-        <v>1.267439174558824</v>
+        <v>1.267439074313726</v>
       </c>
       <c r="P10">
-        <v>1.311003291656863</v>
+        <v>1.311003162</v>
       </c>
       <c r="Q10">
-        <v>1.376529373529412</v>
+        <v>1.37652924754902</v>
       </c>
       <c r="R10">
-        <v>1.437016518823529</v>
+        <v>1.437016422843137</v>
       </c>
       <c r="S10">
-        <v>1.442529796470588</v>
+        <v>1.442529700588235</v>
       </c>
       <c r="T10">
-        <v>1.486636017647059</v>
+        <v>1.48663592254902</v>
       </c>
       <c r="U10">
-        <v>1.517507340882353</v>
+        <v>1.517507258039215</v>
       </c>
       <c r="V10">
-        <v>1.525218855882353</v>
+        <v>1.525218800490196</v>
       </c>
       <c r="W10">
-        <v>1.530727080882353</v>
+        <v>1.530727045098039</v>
       </c>
       <c r="X10">
         <v>2048</v>
@@ -1626,40 +1626,40 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>1.285780789019608</v>
+        <v>1.285780694362745</v>
       </c>
       <c r="M11">
-        <v>1.289737726470588</v>
+        <v>1.289737636078432</v>
       </c>
       <c r="N11">
-        <v>1.295277438901961</v>
+        <v>1.295277354480392</v>
       </c>
       <c r="O11">
-        <v>1.327019174558824</v>
+        <v>1.327019074313726</v>
       </c>
       <c r="P11">
-        <v>1.374007291656863</v>
+        <v>1.374007162</v>
       </c>
       <c r="Q11">
-        <v>1.460264373529412</v>
+        <v>1.46026424754902</v>
       </c>
       <c r="R11">
-        <v>1.53909851882353</v>
+        <v>1.539098422843138</v>
       </c>
       <c r="S11">
-        <v>1.544713796470588</v>
+        <v>1.544713700588235</v>
       </c>
       <c r="T11">
-        <v>1.589636017647059</v>
+        <v>1.58963592254902</v>
       </c>
       <c r="U11">
-        <v>1.624560340882353</v>
+        <v>1.624560258039216</v>
       </c>
       <c r="V11">
-        <v>1.640538855882353</v>
+        <v>1.640538800490196</v>
       </c>
       <c r="W11">
-        <v>1.651952080882353</v>
+        <v>1.651952045098039</v>
       </c>
       <c r="X11">
         <v>2049</v>
@@ -1733,40 +1733,40 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>1.233973289019608</v>
+        <v>1.233973194362745</v>
       </c>
       <c r="M12">
-        <v>1.237592726470588</v>
+        <v>1.237592636078432</v>
       </c>
       <c r="N12">
-        <v>1.242659938901961</v>
+        <v>1.242659854480392</v>
       </c>
       <c r="O12">
-        <v>1.272244174558824</v>
+        <v>1.272244074313726</v>
       </c>
       <c r="P12">
-        <v>1.316104291656863</v>
+        <v>1.316104162</v>
       </c>
       <c r="Q12">
-        <v>1.381824373529412</v>
+        <v>1.38182424754902</v>
       </c>
       <c r="R12">
-        <v>1.442519518823529</v>
+        <v>1.442519422843137</v>
       </c>
       <c r="S12">
-        <v>1.448078296470588</v>
+        <v>1.448078200588235</v>
       </c>
       <c r="T12">
-        <v>1.492548517647059</v>
+        <v>1.49254842254902</v>
       </c>
       <c r="U12">
-        <v>1.523626340882353</v>
+        <v>1.523626258039216</v>
       </c>
       <c r="V12">
-        <v>1.531288855882353</v>
+        <v>1.531288800490196</v>
       </c>
       <c r="W12">
-        <v>1.536762080882353</v>
+        <v>1.53676204509804</v>
       </c>
       <c r="X12">
         <v>2048</v>
@@ -1840,40 +1840,40 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>1.261653289019607</v>
+        <v>1.261653194362745</v>
       </c>
       <c r="M13">
-        <v>1.265592726470588</v>
+        <v>1.265592636078431</v>
       </c>
       <c r="N13">
-        <v>1.271107938901961</v>
+        <v>1.271107854480392</v>
       </c>
       <c r="O13">
-        <v>1.302179174558824</v>
+        <v>1.302179074313726</v>
       </c>
       <c r="P13">
-        <v>1.348111291656863</v>
+        <v>1.348111162</v>
       </c>
       <c r="Q13">
-        <v>1.416934373529412</v>
+        <v>1.41693424754902</v>
       </c>
       <c r="R13">
-        <v>1.481424518823529</v>
+        <v>1.481424422843137</v>
       </c>
       <c r="S13">
-        <v>1.487400796470588</v>
+        <v>1.487400700588235</v>
       </c>
       <c r="T13">
-        <v>1.535211017647059</v>
+        <v>1.53521092254902</v>
       </c>
       <c r="U13">
-        <v>1.567951840882353</v>
+        <v>1.567951758039216</v>
       </c>
       <c r="V13">
-        <v>1.574623855882353</v>
+        <v>1.574623800490196</v>
       </c>
       <c r="W13">
-        <v>1.579389580882353</v>
+        <v>1.579389545098039</v>
       </c>
       <c r="X13">
         <v>2048</v>

</xml_diff>

<commit_message>
Revert "Fix error with exclude column in the meta output by running with --update-expected-files"
This reverts commit 16a14916092996478d10ea045f9dd8cda9b96c4f.
</commit_message>
<xml_diff>
--- a/tests/test-data/workflow-ciceroscm-slimmed/ex2_full_exceedance_probabilities.xlsx
+++ b/tests/test-data/workflow-ciceroscm-slimmed/ex2_full_exceedance_probabilities.xlsx
@@ -663,40 +663,40 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1.261653194362745</v>
+        <v>1.261653289019607</v>
       </c>
       <c r="M2">
-        <v>1.265592636078431</v>
+        <v>1.265592726470588</v>
       </c>
       <c r="N2">
-        <v>1.271107854480392</v>
+        <v>1.271107938901961</v>
       </c>
       <c r="O2">
-        <v>1.302179074313726</v>
+        <v>1.302179174558824</v>
       </c>
       <c r="P2">
-        <v>1.348111162</v>
+        <v>1.348111291656863</v>
       </c>
       <c r="Q2">
-        <v>1.41693424754902</v>
+        <v>1.416934373529412</v>
       </c>
       <c r="R2">
-        <v>1.481424422843137</v>
+        <v>1.481424518823529</v>
       </c>
       <c r="S2">
-        <v>1.487400700588235</v>
+        <v>1.487400796470588</v>
       </c>
       <c r="T2">
-        <v>1.53521092254902</v>
+        <v>1.535211017647059</v>
       </c>
       <c r="U2">
-        <v>1.567951758039216</v>
+        <v>1.567951840882353</v>
       </c>
       <c r="V2">
-        <v>1.574623800490196</v>
+        <v>1.574623855882353</v>
       </c>
       <c r="W2">
-        <v>1.579389545098039</v>
+        <v>1.579389580882353</v>
       </c>
       <c r="X2">
         <v>2048</v>
@@ -770,40 +770,40 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>1.260918194362745</v>
+        <v>1.260918289019608</v>
       </c>
       <c r="M3">
-        <v>1.264802636078432</v>
+        <v>1.264802726470588</v>
       </c>
       <c r="N3">
-        <v>1.270240854480392</v>
+        <v>1.270240938901961</v>
       </c>
       <c r="O3">
-        <v>1.301221574313726</v>
+        <v>1.301221674558824</v>
       </c>
       <c r="P3">
-        <v>1.347061662</v>
+        <v>1.347061791656863</v>
       </c>
       <c r="Q3">
-        <v>1.41583924754902</v>
+        <v>1.415839373529412</v>
       </c>
       <c r="R3">
-        <v>1.480130422843137</v>
+        <v>1.480130518823529</v>
       </c>
       <c r="S3">
-        <v>1.486067700588236</v>
+        <v>1.486067796470588</v>
       </c>
       <c r="T3">
-        <v>1.53356592254902</v>
+        <v>1.533566017647059</v>
       </c>
       <c r="U3">
-        <v>1.566243758039216</v>
+        <v>1.566243840882353</v>
       </c>
       <c r="V3">
-        <v>1.573223800490196</v>
+        <v>1.573223855882353</v>
       </c>
       <c r="W3">
-        <v>1.578209545098039</v>
+        <v>1.578209580882353</v>
       </c>
       <c r="X3">
         <v>2040</v>
@@ -877,40 +877,40 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>1.256278194362745</v>
+        <v>1.256278289019608</v>
       </c>
       <c r="M4">
-        <v>1.260012636078431</v>
+        <v>1.260012726470588</v>
       </c>
       <c r="N4">
-        <v>1.265240854480392</v>
+        <v>1.265240938901961</v>
       </c>
       <c r="O4">
-        <v>1.295456574313726</v>
+        <v>1.295456674558824</v>
       </c>
       <c r="P4">
-        <v>1.340216662</v>
+        <v>1.340216791656863</v>
       </c>
       <c r="Q4">
-        <v>1.40795424754902</v>
+        <v>1.407954373529412</v>
       </c>
       <c r="R4">
-        <v>1.471799422843138</v>
+        <v>1.47179951882353</v>
       </c>
       <c r="S4">
-        <v>1.477678200588236</v>
+        <v>1.477678296470588</v>
       </c>
       <c r="T4">
-        <v>1.52470842254902</v>
+        <v>1.524708517647059</v>
       </c>
       <c r="U4">
-        <v>1.557156758039216</v>
+        <v>1.557156840882353</v>
       </c>
       <c r="V4">
-        <v>1.564283800490196</v>
+        <v>1.564283855882353</v>
       </c>
       <c r="W4">
-        <v>1.569374545098039</v>
+        <v>1.569374580882353</v>
       </c>
       <c r="X4">
         <v>2038</v>
@@ -984,40 +984,40 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>1.278835694362745</v>
+        <v>1.278835789019608</v>
       </c>
       <c r="M5">
-        <v>1.282857636078431</v>
+        <v>1.282857726470588</v>
       </c>
       <c r="N5">
-        <v>1.288488354480392</v>
+        <v>1.288488438901961</v>
       </c>
       <c r="O5">
-        <v>1.320071574313726</v>
+        <v>1.320071674558824</v>
       </c>
       <c r="P5">
-        <v>1.366743662</v>
+        <v>1.366743791656863</v>
       </c>
       <c r="Q5">
-        <v>1.43647924754902</v>
+        <v>1.436479373529412</v>
       </c>
       <c r="R5">
-        <v>1.502008422843137</v>
+        <v>1.50200851882353</v>
       </c>
       <c r="S5">
-        <v>1.508113700588235</v>
+        <v>1.508113796470588</v>
       </c>
       <c r="T5">
-        <v>1.55695592254902</v>
+        <v>1.556956017647059</v>
       </c>
       <c r="U5">
-        <v>1.590257758039216</v>
+        <v>1.590257840882353</v>
       </c>
       <c r="V5">
-        <v>1.596733800490196</v>
+        <v>1.596733855882353</v>
       </c>
       <c r="W5">
-        <v>1.601359545098039</v>
+        <v>1.601359580882353</v>
       </c>
       <c r="X5">
         <v>2048</v>
@@ -1091,40 +1091,40 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>1.256278194362745</v>
+        <v>1.256278289019608</v>
       </c>
       <c r="M6">
-        <v>1.260012636078431</v>
+        <v>1.260012726470588</v>
       </c>
       <c r="N6">
-        <v>1.265240854480392</v>
+        <v>1.265240938901961</v>
       </c>
       <c r="O6">
-        <v>1.295456574313726</v>
+        <v>1.295456674558824</v>
       </c>
       <c r="P6">
-        <v>1.340216662</v>
+        <v>1.340216791656863</v>
       </c>
       <c r="Q6">
-        <v>1.40795424754902</v>
+        <v>1.407954373529412</v>
       </c>
       <c r="R6">
-        <v>1.471799422843138</v>
+        <v>1.47179951882353</v>
       </c>
       <c r="S6">
-        <v>1.477678200588236</v>
+        <v>1.477678296470588</v>
       </c>
       <c r="T6">
-        <v>1.52470842254902</v>
+        <v>1.524708517647059</v>
       </c>
       <c r="U6">
-        <v>1.557156758039216</v>
+        <v>1.557156840882353</v>
       </c>
       <c r="V6">
-        <v>1.564283800490196</v>
+        <v>1.564283855882353</v>
       </c>
       <c r="W6">
-        <v>1.569374545098039</v>
+        <v>1.569374580882353</v>
       </c>
       <c r="X6">
         <v>2038</v>
@@ -1198,40 +1198,40 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>1.256523194362745</v>
+        <v>1.256523289019608</v>
       </c>
       <c r="M7">
-        <v>1.260612636078431</v>
+        <v>1.260612726470588</v>
       </c>
       <c r="N7">
-        <v>1.266337854480392</v>
+        <v>1.266337938901961</v>
       </c>
       <c r="O7">
-        <v>1.298519074313726</v>
+        <v>1.298519174558824</v>
       </c>
       <c r="P7">
-        <v>1.346083162</v>
+        <v>1.346083291656863</v>
       </c>
       <c r="Q7">
-        <v>1.41790424754902</v>
+        <v>1.417904373529412</v>
       </c>
       <c r="R7">
-        <v>1.486979422843137</v>
+        <v>1.48697951882353</v>
       </c>
       <c r="S7">
-        <v>1.493458200588236</v>
+        <v>1.493458296470588</v>
       </c>
       <c r="T7">
-        <v>1.54528842254902</v>
+        <v>1.545288517647059</v>
       </c>
       <c r="U7">
-        <v>1.580195258039216</v>
+        <v>1.580195340882353</v>
       </c>
       <c r="V7">
-        <v>1.586058800490196</v>
+        <v>1.586058855882353</v>
       </c>
       <c r="W7">
-        <v>1.590247045098039</v>
+        <v>1.590247080882353</v>
       </c>
       <c r="X7">
         <v>2040</v>
@@ -1305,40 +1305,40 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>1.347638194362745</v>
+        <v>1.347640789019608</v>
       </c>
       <c r="M8">
-        <v>1.352422636078431</v>
+        <v>1.352427726470588</v>
       </c>
       <c r="N8">
-        <v>1.359120854480392</v>
+        <v>1.359129438901961</v>
       </c>
       <c r="O8">
-        <v>1.394119074313725</v>
+        <v>1.394126674558823</v>
       </c>
       <c r="P8">
-        <v>1.445523162</v>
+        <v>1.445526791656863</v>
       </c>
       <c r="Q8">
-        <v>1.52158924754902</v>
+        <v>1.521589373529412</v>
       </c>
       <c r="R8">
-        <v>1.596046422843137</v>
+        <v>1.596046518823529</v>
       </c>
       <c r="S8">
-        <v>1.603274700588235</v>
+        <v>1.603274796470588</v>
       </c>
       <c r="T8">
-        <v>1.66110092254902</v>
+        <v>1.661101017647059</v>
       </c>
       <c r="U8">
-        <v>1.698780258039216</v>
+        <v>1.698780340882353</v>
       </c>
       <c r="V8">
-        <v>1.702368800490196</v>
+        <v>1.702368855882353</v>
       </c>
       <c r="W8">
-        <v>1.704932045098039</v>
+        <v>1.704932080882353</v>
       </c>
       <c r="X8">
         <v>2048</v>
@@ -1412,40 +1412,40 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>1.229325694362745</v>
+        <v>1.229325789019608</v>
       </c>
       <c r="M9">
-        <v>1.232957636078432</v>
+        <v>1.232957726470588</v>
       </c>
       <c r="N9">
-        <v>1.238042354480392</v>
+        <v>1.238042438901961</v>
       </c>
       <c r="O9">
-        <v>1.267449074313725</v>
+        <v>1.267449174558823</v>
       </c>
       <c r="P9">
-        <v>1.311013162</v>
+        <v>1.311013291656863</v>
       </c>
       <c r="Q9">
-        <v>1.37653924754902</v>
+        <v>1.376539373529412</v>
       </c>
       <c r="R9">
-        <v>1.437029422843137</v>
+        <v>1.437029518823529</v>
       </c>
       <c r="S9">
-        <v>1.442543200588235</v>
+        <v>1.442543296470588</v>
       </c>
       <c r="T9">
-        <v>1.48665342254902</v>
+        <v>1.486653517647059</v>
       </c>
       <c r="U9">
-        <v>1.517525758039216</v>
+        <v>1.517525840882353</v>
       </c>
       <c r="V9">
-        <v>1.525233800490196</v>
+        <v>1.525233855882353</v>
       </c>
       <c r="W9">
-        <v>1.530739545098039</v>
+        <v>1.530739580882353</v>
       </c>
       <c r="X9">
         <v>2048</v>
@@ -1519,40 +1519,40 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>1.229315694362745</v>
+        <v>1.229315789019608</v>
       </c>
       <c r="M10">
-        <v>1.232947636078431</v>
+        <v>1.232947726470588</v>
       </c>
       <c r="N10">
-        <v>1.238032354480392</v>
+        <v>1.238032438901961</v>
       </c>
       <c r="O10">
-        <v>1.267439074313726</v>
+        <v>1.267439174558824</v>
       </c>
       <c r="P10">
-        <v>1.311003162</v>
+        <v>1.311003291656863</v>
       </c>
       <c r="Q10">
-        <v>1.37652924754902</v>
+        <v>1.376529373529412</v>
       </c>
       <c r="R10">
-        <v>1.437016422843137</v>
+        <v>1.437016518823529</v>
       </c>
       <c r="S10">
-        <v>1.442529700588235</v>
+        <v>1.442529796470588</v>
       </c>
       <c r="T10">
-        <v>1.48663592254902</v>
+        <v>1.486636017647059</v>
       </c>
       <c r="U10">
-        <v>1.517507258039215</v>
+        <v>1.517507340882353</v>
       </c>
       <c r="V10">
-        <v>1.525218800490196</v>
+        <v>1.525218855882353</v>
       </c>
       <c r="W10">
-        <v>1.530727045098039</v>
+        <v>1.530727080882353</v>
       </c>
       <c r="X10">
         <v>2048</v>
@@ -1626,40 +1626,40 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>1.285780694362745</v>
+        <v>1.285780789019608</v>
       </c>
       <c r="M11">
-        <v>1.289737636078432</v>
+        <v>1.289737726470588</v>
       </c>
       <c r="N11">
-        <v>1.295277354480392</v>
+        <v>1.295277438901961</v>
       </c>
       <c r="O11">
-        <v>1.327019074313726</v>
+        <v>1.327019174558824</v>
       </c>
       <c r="P11">
-        <v>1.374007162</v>
+        <v>1.374007291656863</v>
       </c>
       <c r="Q11">
-        <v>1.46026424754902</v>
+        <v>1.460264373529412</v>
       </c>
       <c r="R11">
-        <v>1.539098422843138</v>
+        <v>1.53909851882353</v>
       </c>
       <c r="S11">
-        <v>1.544713700588235</v>
+        <v>1.544713796470588</v>
       </c>
       <c r="T11">
-        <v>1.58963592254902</v>
+        <v>1.589636017647059</v>
       </c>
       <c r="U11">
-        <v>1.624560258039216</v>
+        <v>1.624560340882353</v>
       </c>
       <c r="V11">
-        <v>1.640538800490196</v>
+        <v>1.640538855882353</v>
       </c>
       <c r="W11">
-        <v>1.651952045098039</v>
+        <v>1.651952080882353</v>
       </c>
       <c r="X11">
         <v>2049</v>
@@ -1733,40 +1733,40 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>1.233973194362745</v>
+        <v>1.233973289019608</v>
       </c>
       <c r="M12">
-        <v>1.237592636078432</v>
+        <v>1.237592726470588</v>
       </c>
       <c r="N12">
-        <v>1.242659854480392</v>
+        <v>1.242659938901961</v>
       </c>
       <c r="O12">
-        <v>1.272244074313726</v>
+        <v>1.272244174558824</v>
       </c>
       <c r="P12">
-        <v>1.316104162</v>
+        <v>1.316104291656863</v>
       </c>
       <c r="Q12">
-        <v>1.38182424754902</v>
+        <v>1.381824373529412</v>
       </c>
       <c r="R12">
-        <v>1.442519422843137</v>
+        <v>1.442519518823529</v>
       </c>
       <c r="S12">
-        <v>1.448078200588235</v>
+        <v>1.448078296470588</v>
       </c>
       <c r="T12">
-        <v>1.49254842254902</v>
+        <v>1.492548517647059</v>
       </c>
       <c r="U12">
-        <v>1.523626258039216</v>
+        <v>1.523626340882353</v>
       </c>
       <c r="V12">
-        <v>1.531288800490196</v>
+        <v>1.531288855882353</v>
       </c>
       <c r="W12">
-        <v>1.53676204509804</v>
+        <v>1.536762080882353</v>
       </c>
       <c r="X12">
         <v>2048</v>
@@ -1840,40 +1840,40 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>1.261653194362745</v>
+        <v>1.261653289019607</v>
       </c>
       <c r="M13">
-        <v>1.265592636078431</v>
+        <v>1.265592726470588</v>
       </c>
       <c r="N13">
-        <v>1.271107854480392</v>
+        <v>1.271107938901961</v>
       </c>
       <c r="O13">
-        <v>1.302179074313726</v>
+        <v>1.302179174558824</v>
       </c>
       <c r="P13">
-        <v>1.348111162</v>
+        <v>1.348111291656863</v>
       </c>
       <c r="Q13">
-        <v>1.41693424754902</v>
+        <v>1.416934373529412</v>
       </c>
       <c r="R13">
-        <v>1.481424422843137</v>
+        <v>1.481424518823529</v>
       </c>
       <c r="S13">
-        <v>1.487400700588235</v>
+        <v>1.487400796470588</v>
       </c>
       <c r="T13">
-        <v>1.53521092254902</v>
+        <v>1.535211017647059</v>
       </c>
       <c r="U13">
-        <v>1.567951758039216</v>
+        <v>1.567951840882353</v>
       </c>
       <c r="V13">
-        <v>1.574623800490196</v>
+        <v>1.574623855882353</v>
       </c>
       <c r="W13">
-        <v>1.579389545098039</v>
+        <v>1.579389580882353</v>
       </c>
       <c r="X13">
         <v>2048</v>

</xml_diff>